<commit_message>
Feature: Global comments that do not apply to a specific task
</commit_message>
<xml_diff>
--- a/examples/ExampleSheet.xlsx
+++ b/examples/ExampleSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lk/Research/REPOS/assignment-tool/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08D7F27-5322-434D-A1EF-EA4EF39605A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72211487-23F2-5440-81EE-D811D19F5BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="12380" windowWidth="20120" windowHeight="12820" xr2:uid="{7E46A2F1-DF39-B042-96B1-577D7886D6D3}"/>
+    <workbookView xWindow="6020" yWindow="9820" windowWidth="14040" windowHeight="12100" activeTab="2" xr2:uid="{7E46A2F1-DF39-B042-96B1-577D7886D6D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Grading!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="106" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="36">
   <si>
     <t>Username</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>max.pax@student.uni-musterhausen.de</t>
+  </si>
+  <si>
+    <t>You did better this time! Keep going!</t>
+  </si>
+  <si>
+    <t>Please do not submit handwritten solutions in the future.</t>
   </si>
 </sst>
 </file>
@@ -2987,7 +2993,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{71CBA692-DDE1-AE40-A4A7-3756F04DAE0B}" name="PivotTable1" cacheId="106" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{71CBA692-DDE1-AE40-A4A7-3756F04DAE0B}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -3469,7 +3475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DCAF06F-6D54-9944-A4FD-44DA82E6BE85}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3811,9 +3817,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2EEC12-CDA6-A646-9ACB-5F4CBAD98770}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4190,22 +4196,18 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
       <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -4219,7 +4221,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -4239,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -4256,10 +4258,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
@@ -4279,7 +4281,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -4299,13 +4301,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4319,13 +4321,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4342,10 +4344,10 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -4356,16 +4358,16 @@
         <v>1</v>
       </c>
       <c r="C27" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1.5</v>
+        <v>15</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4379,13 +4381,13 @@
         <v>3</v>
       </c>
       <c r="D28" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4399,13 +4401,13 @@
         <v>3</v>
       </c>
       <c r="D29" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4416,16 +4418,16 @@
         <v>1</v>
       </c>
       <c r="C30" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="6">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4439,13 +4441,13 @@
         <v>4</v>
       </c>
       <c r="D31" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -4459,13 +4461,13 @@
         <v>4</v>
       </c>
       <c r="D32" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -4479,13 +4481,13 @@
         <v>4</v>
       </c>
       <c r="D33" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="6">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -4499,33 +4501,33 @@
         <v>4</v>
       </c>
       <c r="D34" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="6">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
       </c>
       <c r="C35" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -4539,13 +4541,13 @@
         <v>1</v>
       </c>
       <c r="D36" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -4559,13 +4561,13 @@
         <v>1</v>
       </c>
       <c r="D37" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -4576,16 +4578,16 @@
         <v>1</v>
       </c>
       <c r="C38" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
       <c r="F38" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -4599,13 +4601,13 @@
         <v>2</v>
       </c>
       <c r="D39" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4619,7 +4621,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40" t="s">
         <v>14</v>
@@ -4639,7 +4641,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
@@ -4656,16 +4658,16 @@
         <v>1</v>
       </c>
       <c r="C42" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -4679,13 +4681,13 @@
         <v>3</v>
       </c>
       <c r="D43" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -4699,13 +4701,13 @@
         <v>3</v>
       </c>
       <c r="D44" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
       </c>
       <c r="F44" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -4716,16 +4718,16 @@
         <v>1</v>
       </c>
       <c r="C45" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -4739,13 +4741,13 @@
         <v>4</v>
       </c>
       <c r="D46" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
       </c>
       <c r="F46" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -4759,7 +4761,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
@@ -4779,13 +4781,13 @@
         <v>4</v>
       </c>
       <c r="D48" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
       </c>
       <c r="F48" s="6">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -4799,13 +4801,13 @@
         <v>4</v>
       </c>
       <c r="D49" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
       </c>
       <c r="F49" s="6">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -4822,10 +4824,45 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6">
+        <v>4</v>
+      </c>
+      <c r="D51" s="6">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
         <v>15</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4838,7 +4875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F790B2-0695-184C-B2AB-3640E6DE5875}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>